<commit_message>
Work on the tests and explanation of algorithms
</commit_message>
<xml_diff>
--- a/_Writeup/Test Plan Organisation.xlsx
+++ b/_Writeup/Test Plan Organisation.xlsx
@@ -342,18 +342,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -374,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,10 +377,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +832,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="8">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1060,7 +1053,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="8">
         <f>B43+1</f>
         <v>35</v>
@@ -1070,7 +1063,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="8">
         <f>B44+1</f>
         <v>36</v>
@@ -1330,7 +1323,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="8">
         <f>B71+1</f>
         <v>63</v>
@@ -1378,7 +1371,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+      <c r="A77" s="1"/>
       <c r="B77" s="8">
         <f t="shared" si="7"/>
         <v>68</v>
@@ -1388,7 +1381,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
+      <c r="A78" s="9"/>
       <c r="B78" s="8">
         <f t="shared" si="7"/>
         <v>69</v>
@@ -1402,7 +1395,7 @@
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
+      <c r="A80" s="9"/>
       <c r="B80" s="8">
         <f>B78+1</f>
         <v>70</v>
@@ -1492,7 +1485,7 @@
       <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="11"/>
+      <c r="A91" s="9"/>
       <c r="B91" s="8">
         <f>B89+1</f>
         <v>79</v>

</xml_diff>